<commit_message>
Improved benchmark source code
</commit_message>
<xml_diff>
--- a/doc/performance.xlsx
+++ b/doc/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mueller/data/bau/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D107C0A1-8D42-F142-B3B8-BCB98DAFA76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B0ADE3-DD76-9C40-ACA1-BA17D27D9C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21400" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -1408,16 +1408,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>232</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5578</c:v>
+                  <c:v>5594</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2145</c:v>
+                  <c:v>2176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2695</c:v>
+                  <c:v>2684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,16 +1479,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>236</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5577</c:v>
+                  <c:v>5627</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2121</c:v>
+                  <c:v>2144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2807</c:v>
+                  <c:v>2829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,16 +1550,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>296</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6589</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2573</c:v>
+                  <c:v>2546</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3181</c:v>
+                  <c:v>3211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1692,16 +1692,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>315</c:v>
+                  <c:v>307</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7442</c:v>
+                  <c:v>7283</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2676</c:v>
+                  <c:v>2611</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3559</c:v>
+                  <c:v>3477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1763,16 +1763,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>343</c:v>
+                  <c:v>336</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7337</c:v>
+                  <c:v>7237</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2860</c:v>
+                  <c:v>2783</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3286</c:v>
+                  <c:v>3268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,25 +2141,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0172413793103448</c:v>
+                  <c:v>1.0214592274678111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2758620689655171</c:v>
+                  <c:v>1.2145922746781115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1939655172413792</c:v>
+                  <c:v>1.1888412017167382</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3577586206896552</c:v>
+                  <c:v>1.3175965665236051</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.478448275862069</c:v>
+                  <c:v>1.4420600858369099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2413793103448276</c:v>
+                  <c:v>1.1931330472103003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4655172413793103</c:v>
+                  <c:v>1.4592274678111588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,25 +2236,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99982072427393343</c:v>
+                  <c:v>1.0058991776903825</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1812477590534243</c:v>
+                  <c:v>1.1778691455130497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2465041233416996</c:v>
+                  <c:v>1.2429388630675724</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3341699533883113</c:v>
+                  <c:v>1.3019306399713979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3153460021513088</c:v>
+                  <c:v>1.2937075437969252</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4560774471136608</c:v>
+                  <c:v>1.419377904898105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4888849049838653</c:v>
+                  <c:v>1.4839113335716838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2331,25 +2331,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98881118881118879</c:v>
+                  <c:v>0.98529411764705876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1995337995337996</c:v>
+                  <c:v>1.1700367647058822</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2074592074592074</c:v>
+                  <c:v>1.1902573529411764</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2475524475524475</c:v>
+                  <c:v>1.1999080882352942</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3333333333333333</c:v>
+                  <c:v>1.278952205882353</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6181818181818182</c:v>
+                  <c:v>1.5266544117647058</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5426573426573427</c:v>
+                  <c:v>1.5206801470588236</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2426,25 +2426,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0415584415584416</c:v>
+                  <c:v>1.0540238450074515</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1803339517625231</c:v>
+                  <c:v>1.1963487332339791</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2990723562152133</c:v>
+                  <c:v>1.3043964232488823</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3205936920222634</c:v>
+                  <c:v>1.2954545454545454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2192949907235622</c:v>
+                  <c:v>1.2175856929955291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3473098330241187</c:v>
+                  <c:v>1.3438897168405366</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3673469387755102</c:v>
+                  <c:v>1.3729508196721312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2521,25 +2521,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95139911634756991</c:v>
+                  <c:v>0.95876288659793818</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2164948453608246</c:v>
+                  <c:v>1.2120765832106037</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.2739322533136965</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6774668630338734</c:v>
+                  <c:v>1.6597938144329896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5139911634756995</c:v>
+                  <c:v>1.5066273932253313</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5007363770250368</c:v>
+                  <c:v>1.4874815905743741</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8350515463917525</c:v>
+                  <c:v>1.829160530191458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2591,7 +2591,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5283,7 +5283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCE9842-6C14-0245-8092-DD3DC9C4F639}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D32"/>
     </sheetView>
   </sheetViews>
@@ -6122,7 +6122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCA3CD0-A1E2-3843-9734-943657D6AF5A}">
   <dimension ref="B2:N74"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -6171,16 +6171,16 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D3">
-        <v>5578</v>
+        <v>5594</v>
       </c>
       <c r="E3">
-        <v>2145</v>
+        <v>2176</v>
       </c>
       <c r="F3">
-        <v>2695</v>
+        <v>2684</v>
       </c>
       <c r="G3">
         <v>679</v>
@@ -6215,19 +6215,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D4">
-        <v>5577</v>
+        <v>5627</v>
       </c>
       <c r="E4">
-        <v>2121</v>
+        <v>2144</v>
       </c>
       <c r="F4">
-        <v>2807</v>
+        <v>2829</v>
       </c>
       <c r="G4">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="I4" s="4" t="str">
         <f t="shared" ref="I4:I10" si="4">B4</f>
@@ -6235,23 +6235,23 @@
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J8" si="5">1/C$3*C4</f>
-        <v>1.0172413793103448</v>
+        <v>1.0214592274678111</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0.99982072427393343</v>
+        <v>1.0058991776903825</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>0.98881118881118879</v>
+        <v>0.98529411764705876</v>
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
-        <v>1.0415584415584416</v>
+        <v>1.0540238450074515</v>
       </c>
       <c r="N4">
         <f t="shared" si="3"/>
-        <v>0.95139911634756991</v>
+        <v>0.95876288659793818</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -6259,19 +6259,19 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="D5">
         <v>6589</v>
       </c>
       <c r="E5">
-        <v>2573</v>
+        <v>2546</v>
       </c>
       <c r="F5">
-        <v>3181</v>
+        <v>3211</v>
       </c>
       <c r="G5">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6279,23 +6279,23 @@
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
-        <v>1.2758620689655171</v>
+        <v>1.2145922746781115</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>1.1812477590534243</v>
+        <v>1.1778691455130497</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>1.1995337995337996</v>
+        <v>1.1700367647058822</v>
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>1.1803339517625231</v>
+        <v>1.1963487332339791</v>
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
-        <v>1.2164948453608246</v>
+        <v>1.2120765832106037</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
@@ -6323,19 +6323,19 @@
       </c>
       <c r="J6">
         <f t="shared" si="5"/>
-        <v>1.1939655172413792</v>
+        <v>1.1888412017167382</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>1.2465041233416996</v>
+        <v>1.2429388630675724</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>1.2074592074592074</v>
+        <v>1.1902573529411764</v>
       </c>
       <c r="M6">
         <f t="shared" si="2"/>
-        <v>1.2990723562152133</v>
+        <v>1.3043964232488823</v>
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
@@ -6347,19 +6347,19 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D7">
-        <v>7442</v>
+        <v>7283</v>
       </c>
       <c r="E7">
-        <v>2676</v>
+        <v>2611</v>
       </c>
       <c r="F7">
-        <v>3559</v>
+        <v>3477</v>
       </c>
       <c r="G7">
-        <v>1139</v>
+        <v>1127</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6367,23 +6367,23 @@
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>1.3577586206896552</v>
+        <v>1.3175965665236051</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1.3341699533883113</v>
+        <v>1.3019306399713979</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>1.2475524475524475</v>
+        <v>1.1999080882352942</v>
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>1.3205936920222634</v>
+        <v>1.2954545454545454</v>
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>1.6774668630338734</v>
+        <v>1.6597938144329896</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -6391,19 +6391,19 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D8">
-        <v>7337</v>
+        <v>7237</v>
       </c>
       <c r="E8">
-        <v>2860</v>
+        <v>2783</v>
       </c>
       <c r="F8">
-        <v>3286</v>
+        <v>3268</v>
       </c>
       <c r="G8">
-        <v>1028</v>
+        <v>1023</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6411,23 +6411,23 @@
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>1.478448275862069</v>
+        <v>1.4420600858369099</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>1.3153460021513088</v>
+        <v>1.2937075437969252</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
+        <v>1.278952205882353</v>
       </c>
       <c r="M8">
         <f t="shared" si="2"/>
-        <v>1.2192949907235622</v>
+        <v>1.2175856929955291</v>
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>1.5139911634756995</v>
+        <v>1.5066273932253313</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -6435,19 +6435,19 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D9" s="3">
-        <v>8122</v>
+        <v>7940</v>
       </c>
       <c r="E9">
-        <v>3471</v>
+        <v>3322</v>
       </c>
       <c r="F9">
-        <v>3631</v>
+        <v>3607</v>
       </c>
       <c r="G9">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6455,23 +6455,23 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9" si="6">1/C$3*C9</f>
-        <v>1.2413793103448276</v>
+        <v>1.1931330472103003</v>
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K10" si="7">1/D$3*D9</f>
-        <v>1.4560774471136608</v>
+        <v>1.419377904898105</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L10" si="8">1/E$3*E9</f>
-        <v>1.6181818181818182</v>
+        <v>1.5266544117647058</v>
       </c>
       <c r="M9">
         <f t="shared" ref="M9:M10" si="9">1/F$3*F9</f>
-        <v>1.3473098330241187</v>
+        <v>1.3438897168405366</v>
       </c>
       <c r="N9">
         <f t="shared" ref="N9:N10" si="10">1/G$3*G9</f>
-        <v>1.5007363770250368</v>
+        <v>1.4874815905743741</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -6482,7 +6482,7 @@
         <v>340</v>
       </c>
       <c r="D10" s="3">
-        <v>8305</v>
+        <v>8301</v>
       </c>
       <c r="E10">
         <v>3309</v>
@@ -6491,7 +6491,7 @@
         <v>3685</v>
       </c>
       <c r="G10">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="I10" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6499,23 +6499,23 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10" si="11">1/C$3*C10</f>
-        <v>1.4655172413793103</v>
+        <v>1.4592274678111588</v>
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
-        <v>1.4888849049838653</v>
+        <v>1.4839113335716838</v>
       </c>
       <c r="L10">
         <f t="shared" si="8"/>
-        <v>1.5426573426573427</v>
+        <v>1.5206801470588236</v>
       </c>
       <c r="M10">
         <f t="shared" si="9"/>
-        <v>1.3673469387755102</v>
+        <v>1.3729508196721312</v>
       </c>
       <c r="N10">
         <f t="shared" si="10"/>
-        <v>1.8350515463917525</v>
+        <v>1.829160530191458</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Support initializing multiple variables in one line
</commit_message>
<xml_diff>
--- a/doc/performance.xlsx
+++ b/doc/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mueller/data/bau/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B0ADE3-DD76-9C40-ACA1-BA17D27D9C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC92C038-ECC0-FC4F-90BE-C324AFAA2EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32020" windowHeight="18980" activeTab="2" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -1411,13 +1411,13 @@
                   <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5594</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2684</c:v>
+                  <c:v>2687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,16 +1479,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>238</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5627</c:v>
+                  <c:v>5513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2144</c:v>
+                  <c:v>2064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2829</c:v>
+                  <c:v>2805</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1553,13 +1553,13 @@
                   <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6589</c:v>
+                  <c:v>6564</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2546</c:v>
+                  <c:v>2540</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3211</c:v>
+                  <c:v>3195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1692,16 +1692,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>307</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7283</c:v>
+                  <c:v>7273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2611</c:v>
+                  <c:v>2606</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3477</c:v>
+                  <c:v>3473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1763,16 +1763,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>336</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7237</c:v>
+                  <c:v>7063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2783</c:v>
+                  <c:v>2775</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3268</c:v>
+                  <c:v>3213</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,7 +2141,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0214592274678111</c:v>
+                  <c:v>0.97854077253218885</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.2145922746781115</c:v>
@@ -2150,10 +2150,10 @@
                   <c:v>1.1888412017167382</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3175965665236051</c:v>
+                  <c:v>1.3133047210300428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4420600858369099</c:v>
+                  <c:v>1.4334763948497855</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.1931330472103003</c:v>
@@ -2236,25 +2236,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0058991776903825</c:v>
+                  <c:v>0.98446428571428568</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1778691455130497</c:v>
+                  <c:v>1.1721428571428572</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2429388630675724</c:v>
+                  <c:v>1.2416071428571429</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3019306399713979</c:v>
+                  <c:v>1.2987500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2937075437969252</c:v>
+                  <c:v>1.26125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.419377904898105</c:v>
+                  <c:v>1.4157142857142857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4839113335716838</c:v>
+                  <c:v>1.4823214285714286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2331,19 +2331,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98529411764705876</c:v>
+                  <c:v>0.94852941176470584</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1700367647058822</c:v>
+                  <c:v>1.1672794117647058</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.1902573529411764</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1999080882352942</c:v>
+                  <c:v>1.197610294117647</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.278952205882353</c:v>
+                  <c:v>1.2752757352941175</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.5266544117647058</c:v>
@@ -2426,25 +2426,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0540238450074515</c:v>
+                  <c:v>1.0439151470040939</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1963487332339791</c:v>
+                  <c:v>1.1890584294752513</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3043964232488823</c:v>
+                  <c:v>1.302940081875698</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2954545454545454</c:v>
+                  <c:v>1.2925195385187942</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2175856929955291</c:v>
+                  <c:v>1.1957573502046892</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3438897168405366</c:v>
+                  <c:v>1.3401563081503536</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3729508196721312</c:v>
+                  <c:v>1.3714179382210645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2521,25 +2521,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95876288659793818</c:v>
+                  <c:v>0.93988269794721413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2120765832106037</c:v>
+                  <c:v>1.2023460410557185</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2739322533136965</c:v>
+                  <c:v>1.2683284457478006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6597938144329896</c:v>
+                  <c:v>1.6510263929618769</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5066273932253313</c:v>
+                  <c:v>1.4897360703812317</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4874815905743741</c:v>
+                  <c:v>1.4721407624633431</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.829160530191458</c:v>
+                  <c:v>1.8211143695014662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6122,8 +6122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCA3CD0-A1E2-3843-9734-943657D6AF5A}">
   <dimension ref="B2:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6174,16 +6174,16 @@
         <v>233</v>
       </c>
       <c r="D3">
-        <v>5594</v>
+        <v>5600</v>
       </c>
       <c r="E3">
         <v>2176</v>
       </c>
       <c r="F3">
-        <v>2684</v>
+        <v>2687</v>
       </c>
       <c r="G3">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="I3" s="4" t="str">
         <f>B3</f>
@@ -6215,19 +6215,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D4">
-        <v>5627</v>
+        <v>5513</v>
       </c>
       <c r="E4">
-        <v>2144</v>
+        <v>2064</v>
       </c>
       <c r="F4">
-        <v>2829</v>
+        <v>2805</v>
       </c>
       <c r="G4">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="I4" s="4" t="str">
         <f t="shared" ref="I4:I10" si="4">B4</f>
@@ -6235,23 +6235,23 @@
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J8" si="5">1/C$3*C4</f>
-        <v>1.0214592274678111</v>
+        <v>0.97854077253218885</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>1.0058991776903825</v>
+        <v>0.98446428571428568</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>0.98529411764705876</v>
+        <v>0.94852941176470584</v>
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
-        <v>1.0540238450074515</v>
+        <v>1.0439151470040939</v>
       </c>
       <c r="N4">
         <f t="shared" si="3"/>
-        <v>0.95876288659793818</v>
+        <v>0.93988269794721413</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -6262,16 +6262,16 @@
         <v>283</v>
       </c>
       <c r="D5">
-        <v>6589</v>
+        <v>6564</v>
       </c>
       <c r="E5">
-        <v>2546</v>
+        <v>2540</v>
       </c>
       <c r="F5">
-        <v>3211</v>
+        <v>3195</v>
       </c>
       <c r="G5">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6283,19 +6283,19 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>1.1778691455130497</v>
+        <v>1.1721428571428572</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>1.1700367647058822</v>
+        <v>1.1672794117647058</v>
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>1.1963487332339791</v>
+        <v>1.1890584294752513</v>
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
-        <v>1.2120765832106037</v>
+        <v>1.2023460410557185</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
@@ -6327,7 +6327,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>1.2429388630675724</v>
+        <v>1.2416071428571429</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
@@ -6335,11 +6335,11 @@
       </c>
       <c r="M6">
         <f t="shared" si="2"/>
-        <v>1.3043964232488823</v>
+        <v>1.302940081875698</v>
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>1.2739322533136965</v>
+        <v>1.2683284457478006</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
@@ -6347,19 +6347,19 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D7">
-        <v>7283</v>
+        <v>7273</v>
       </c>
       <c r="E7">
-        <v>2611</v>
+        <v>2606</v>
       </c>
       <c r="F7">
-        <v>3477</v>
+        <v>3473</v>
       </c>
       <c r="G7">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6367,23 +6367,23 @@
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>1.3175965665236051</v>
+        <v>1.3133047210300428</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1.3019306399713979</v>
+        <v>1.2987500000000001</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>1.1999080882352942</v>
+        <v>1.197610294117647</v>
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>1.2954545454545454</v>
+        <v>1.2925195385187942</v>
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>1.6597938144329896</v>
+        <v>1.6510263929618769</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -6391,19 +6391,19 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D8">
-        <v>7237</v>
+        <v>7063</v>
       </c>
       <c r="E8">
-        <v>2783</v>
+        <v>2775</v>
       </c>
       <c r="F8">
-        <v>3268</v>
+        <v>3213</v>
       </c>
       <c r="G8">
-        <v>1023</v>
+        <v>1016</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6411,23 +6411,23 @@
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>1.4420600858369099</v>
+        <v>1.4334763948497855</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>1.2937075437969252</v>
+        <v>1.26125</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>1.278952205882353</v>
+        <v>1.2752757352941175</v>
       </c>
       <c r="M8">
         <f t="shared" si="2"/>
-        <v>1.2175856929955291</v>
+        <v>1.1957573502046892</v>
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>1.5066273932253313</v>
+        <v>1.4897360703812317</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -6438,16 +6438,16 @@
         <v>278</v>
       </c>
       <c r="D9" s="3">
-        <v>7940</v>
+        <v>7928</v>
       </c>
       <c r="E9">
         <v>3322</v>
       </c>
       <c r="F9">
-        <v>3607</v>
+        <v>3601</v>
       </c>
       <c r="G9">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K10" si="7">1/D$3*D9</f>
-        <v>1.419377904898105</v>
+        <v>1.4157142857142857</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L10" si="8">1/E$3*E9</f>
@@ -6467,11 +6467,11 @@
       </c>
       <c r="M9">
         <f t="shared" ref="M9:M10" si="9">1/F$3*F9</f>
-        <v>1.3438897168405366</v>
+        <v>1.3401563081503536</v>
       </c>
       <c r="N9">
         <f t="shared" ref="N9:N10" si="10">1/G$3*G9</f>
-        <v>1.4874815905743741</v>
+        <v>1.4721407624633431</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
-        <v>1.4839113335716838</v>
+        <v>1.4823214285714286</v>
       </c>
       <c r="L10">
         <f t="shared" si="8"/>
@@ -6511,11 +6511,11 @@
       </c>
       <c r="M10">
         <f t="shared" si="9"/>
-        <v>1.3729508196721312</v>
+        <v>1.3714179382210645</v>
       </c>
       <c r="N10">
         <f t="shared" si="10"/>
-        <v>1.829160530191458</v>
+        <v>1.8211143695014662</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Auto-conversion from int to bigInt; Avoid problematic semicolons in C; Fallback for missing __builtin_ctzll; Reduce usage of 'goto' to allow WASM compilation
</commit_message>
<xml_diff>
--- a/doc/performance.xlsx
+++ b/doc/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mueller/data/bau/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC92C038-ECC0-FC4F-90BE-C324AFAA2EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDB66D8-429C-2C49-96DD-CC360912F79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32020" windowHeight="18980" activeTab="2" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -1408,16 +1408,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>233</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5600</c:v>
+                  <c:v>5408</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2176</c:v>
+                  <c:v>2086</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2687</c:v>
+                  <c:v>2595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,16 +1479,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>228</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5513</c:v>
+                  <c:v>5416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2064</c:v>
+                  <c:v>2063</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2805</c:v>
+                  <c:v>2716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1553,10 +1553,10 @@
                   <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6564</c:v>
+                  <c:v>6566</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2540</c:v>
+                  <c:v>2542</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3195</c:v>
@@ -1695,13 +1695,13 @@
                   <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7273</c:v>
+                  <c:v>7268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2606</c:v>
+                  <c:v>2604</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3473</c:v>
+                  <c:v>3477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1766,13 +1766,13 @@
                   <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7063</c:v>
+                  <c:v>7037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2775</c:v>
+                  <c:v>2764</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3213</c:v>
+                  <c:v>3217</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,25 +2141,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97854077253218885</c:v>
+                  <c:v>1.0225225225225225</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2145922746781115</c:v>
+                  <c:v>1.2747747747747749</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1888412017167382</c:v>
+                  <c:v>1.2477477477477477</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3133047210300428</c:v>
+                  <c:v>1.3783783783783783</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4334763948497855</c:v>
+                  <c:v>1.5045045045045045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1931330472103003</c:v>
+                  <c:v>1.2522522522522523</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4592274678111588</c:v>
+                  <c:v>1.5315315315315314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,25 +2236,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98446428571428568</c:v>
+                  <c:v>1.0014792899408285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1721428571428572</c:v>
+                  <c:v>1.2141272189349113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2416071428571429</c:v>
+                  <c:v>1.2856878698224852</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2987500000000001</c:v>
+                  <c:v>1.3439349112426036</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.26125</c:v>
+                  <c:v>1.3012204142011834</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4157142857142857</c:v>
+                  <c:v>1.4659763313609466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4823214285714286</c:v>
+                  <c:v>1.5367973372781065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2331,25 +2331,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94852941176470584</c:v>
+                  <c:v>0.98897411313518691</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1672794117647058</c:v>
+                  <c:v>1.2186001917545541</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1902573529411764</c:v>
+                  <c:v>1.2416107382550334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.197610294117647</c:v>
+                  <c:v>1.2483221476510067</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2752757352941175</c:v>
+                  <c:v>1.3250239693192714</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5266544117647058</c:v>
+                  <c:v>1.592521572387344</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5206801470588236</c:v>
+                  <c:v>1.587248322147651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2426,25 +2426,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0439151470040939</c:v>
+                  <c:v>1.0466281310211947</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1890584294752513</c:v>
+                  <c:v>1.23121387283237</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.302940081875698</c:v>
+                  <c:v>1.3491329479768785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2925195385187942</c:v>
+                  <c:v>1.3398843930635838</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1957573502046892</c:v>
+                  <c:v>1.2396917148362234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3401563081503536</c:v>
+                  <c:v>1.3876685934489403</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3714179382210645</c:v>
+                  <c:v>1.4231213872832371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2521,25 +2521,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93988269794721413</c:v>
+                  <c:v>0.93814432989690721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2023460410557185</c:v>
+                  <c:v>1.2268041237113403</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2683284457478006</c:v>
+                  <c:v>1.2739322533136965</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6510263929618769</c:v>
+                  <c:v>1.6583210603829159</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4897360703812317</c:v>
+                  <c:v>1.5022091310751104</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4721407624633431</c:v>
+                  <c:v>1.4830633284241532</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8211143695014662</c:v>
+                  <c:v>1.8335787923416789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4638,15 +4638,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:colOff>533260</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6122,8 +6122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCA3CD0-A1E2-3843-9734-943657D6AF5A}">
   <dimension ref="B2:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6171,19 +6171,22 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D3">
-        <v>5600</v>
+        <v>5408</v>
       </c>
       <c r="E3">
-        <v>2176</v>
+        <v>2086</v>
       </c>
       <c r="F3">
-        <v>2687</v>
+        <v>2595</v>
       </c>
       <c r="G3">
-        <v>682</v>
+        <v>679</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
       </c>
       <c r="I3" s="4" t="str">
         <f>B3</f>
@@ -6215,19 +6218,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D4">
-        <v>5513</v>
+        <v>5416</v>
       </c>
       <c r="E4">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="F4">
-        <v>2805</v>
+        <v>2716</v>
       </c>
       <c r="G4">
-        <v>641</v>
+        <v>637</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
       <c r="I4" s="4" t="str">
         <f t="shared" ref="I4:I10" si="4">B4</f>
@@ -6235,23 +6241,23 @@
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J8" si="5">1/C$3*C4</f>
-        <v>0.97854077253218885</v>
+        <v>1.0225225225225225</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0.98446428571428568</v>
+        <v>1.0014792899408285</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>0.94852941176470584</v>
+        <v>0.98897411313518691</v>
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
-        <v>1.0439151470040939</v>
+        <v>1.0466281310211947</v>
       </c>
       <c r="N4">
         <f t="shared" si="3"/>
-        <v>0.93988269794721413</v>
+        <v>0.93814432989690721</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -6262,16 +6268,19 @@
         <v>283</v>
       </c>
       <c r="D5">
-        <v>6564</v>
+        <v>6566</v>
       </c>
       <c r="E5">
-        <v>2540</v>
+        <v>2542</v>
       </c>
       <c r="F5">
         <v>3195</v>
       </c>
       <c r="G5">
-        <v>820</v>
+        <v>833</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6279,23 +6288,23 @@
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
-        <v>1.2145922746781115</v>
+        <v>1.2747747747747749</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>1.1721428571428572</v>
+        <v>1.2141272189349113</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>1.1672794117647058</v>
+        <v>1.2186001917545541</v>
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>1.1890584294752513</v>
+        <v>1.23121387283237</v>
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
-        <v>1.2023460410557185</v>
+        <v>1.2268041237113403</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
@@ -6317,29 +6326,32 @@
       <c r="G6">
         <v>865</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Kotlin</v>
       </c>
       <c r="J6">
         <f t="shared" si="5"/>
-        <v>1.1888412017167382</v>
+        <v>1.2477477477477477</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>1.2416071428571429</v>
+        <v>1.2856878698224852</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>1.1902573529411764</v>
+        <v>1.2416107382550334</v>
       </c>
       <c r="M6">
         <f t="shared" si="2"/>
-        <v>1.302940081875698</v>
+        <v>1.3491329479768785</v>
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>1.2683284457478006</v>
+        <v>1.2739322533136965</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
@@ -6350,16 +6362,19 @@
         <v>306</v>
       </c>
       <c r="D7">
-        <v>7273</v>
+        <v>7268</v>
       </c>
       <c r="E7">
-        <v>2606</v>
+        <v>2604</v>
       </c>
       <c r="F7">
-        <v>3473</v>
+        <v>3477</v>
       </c>
       <c r="G7">
         <v>1126</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6367,23 +6382,23 @@
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>1.3133047210300428</v>
+        <v>1.3783783783783783</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1.2987500000000001</v>
+        <v>1.3439349112426036</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>1.197610294117647</v>
+        <v>1.2483221476510067</v>
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>1.2925195385187942</v>
+        <v>1.3398843930635838</v>
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>1.6510263929618769</v>
+        <v>1.6583210603829159</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -6394,16 +6409,19 @@
         <v>334</v>
       </c>
       <c r="D8">
-        <v>7063</v>
+        <v>7037</v>
       </c>
       <c r="E8">
-        <v>2775</v>
+        <v>2764</v>
       </c>
       <c r="F8">
-        <v>3213</v>
+        <v>3217</v>
       </c>
       <c r="G8">
-        <v>1016</v>
+        <v>1020</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6411,23 +6429,23 @@
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>1.4334763948497855</v>
+        <v>1.5045045045045045</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>1.26125</v>
+        <v>1.3012204142011834</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>1.2752757352941175</v>
+        <v>1.3250239693192714</v>
       </c>
       <c r="M8">
         <f t="shared" si="2"/>
-        <v>1.1957573502046892</v>
+        <v>1.2396917148362234</v>
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>1.4897360703812317</v>
+        <v>1.5022091310751104</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -6447,7 +6465,10 @@
         <v>3601</v>
       </c>
       <c r="G9">
-        <v>1004</v>
+        <v>1007</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6455,23 +6476,23 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9" si="6">1/C$3*C9</f>
-        <v>1.1931330472103003</v>
+        <v>1.2522522522522523</v>
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K10" si="7">1/D$3*D9</f>
-        <v>1.4157142857142857</v>
+        <v>1.4659763313609466</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L10" si="8">1/E$3*E9</f>
-        <v>1.5266544117647058</v>
+        <v>1.592521572387344</v>
       </c>
       <c r="M9">
         <f t="shared" ref="M9:M10" si="9">1/F$3*F9</f>
-        <v>1.3401563081503536</v>
+        <v>1.3876685934489403</v>
       </c>
       <c r="N9">
         <f t="shared" ref="N9:N10" si="10">1/G$3*G9</f>
-        <v>1.4721407624633431</v>
+        <v>1.4830633284241532</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -6482,16 +6503,19 @@
         <v>340</v>
       </c>
       <c r="D10" s="3">
-        <v>8301</v>
+        <v>8311</v>
       </c>
       <c r="E10">
-        <v>3309</v>
+        <v>3311</v>
       </c>
       <c r="F10">
-        <v>3685</v>
+        <v>3693</v>
       </c>
       <c r="G10">
-        <v>1242</v>
+        <v>1245</v>
+      </c>
+      <c r="H10">
+        <v>65</v>
       </c>
       <c r="I10" s="4" t="str">
         <f t="shared" si="4"/>
@@ -6499,23 +6523,23 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10" si="11">1/C$3*C10</f>
-        <v>1.4592274678111588</v>
+        <v>1.5315315315315314</v>
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
-        <v>1.4823214285714286</v>
+        <v>1.5367973372781065</v>
       </c>
       <c r="L10">
         <f t="shared" si="8"/>
-        <v>1.5206801470588236</v>
+        <v>1.587248322147651</v>
       </c>
       <c r="M10">
         <f t="shared" si="9"/>
-        <v>1.3714179382210645</v>
+        <v>1.4231213872832371</v>
       </c>
       <c r="N10">
         <f t="shared" si="10"/>
-        <v>1.8211143695014662</v>
+        <v>1.8335787923416789</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Benchmarks: add Nim, V, Zig
</commit_message>
<xml_diff>
--- a/doc/performance.xlsx
+++ b/doc/performance.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mueller/data/bau/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDB66D8-429C-2C49-96DD-CC360912F79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FB8C5C-44B4-C74B-A92F-57BA8C016EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34040" windowHeight="17500" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
-    <sheet name="signal" sheetId="3" r:id="rId2"/>
-    <sheet name="Concise" sheetId="2" r:id="rId3"/>
+    <sheet name="Concise" sheetId="2" r:id="rId2"/>
+    <sheet name="signal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="147">
   <si>
     <t>Benchmark</t>
   </si>
@@ -467,6 +467,18 @@
   </si>
   <si>
     <t>window size changed</t>
+  </si>
+  <si>
+    <t>Underscore</t>
+  </si>
+  <si>
+    <t>Nim</t>
+  </si>
+  <si>
+    <t>Vlang</t>
+  </si>
+  <si>
+    <t>Zig</t>
   </si>
 </sst>
 </file>
@@ -538,8 +550,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,9 +671,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$C$4:$I$4</c:f>
+              <c:f>Performance!$C$4:$L$4</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Bau</c:v>
                 </c:pt>
@@ -675,23 +687,32 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>PyPy</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Rust</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Swift</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$C$5:$I$5</c:f>
+              <c:f>Performance!$C$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.0999999999999996</c:v>
                 </c:pt>
@@ -705,13 +726,22 @@
                   <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>8.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>5.9</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -748,9 +778,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$C$4:$I$4</c:f>
+              <c:f>Performance!$C$4:$L$4</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Bau</c:v>
                 </c:pt>
@@ -764,23 +794,32 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>PyPy</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Rust</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Swift</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$C$6:$I$6</c:f>
+              <c:f>Performance!$C$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.1</c:v>
                 </c:pt>
@@ -794,13 +833,22 @@
                   <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,9 +885,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$C$4:$I$4</c:f>
+              <c:f>Performance!$C$4:$L$4</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Bau</c:v>
                 </c:pt>
@@ -853,23 +901,32 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>PyPy</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Rust</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Swift</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$C$7:$I$7</c:f>
+              <c:f>Performance!$C$7:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -883,13 +940,22 @@
                   <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>15.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.8</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -926,9 +992,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$C$4:$I$4</c:f>
+              <c:f>Performance!$C$4:$L$4</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Bau</c:v>
                 </c:pt>
@@ -942,23 +1008,32 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>PyPy</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Rust</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Swift</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$C$8:$I$8</c:f>
+              <c:f>Performance!$C$8:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.6</c:v>
                 </c:pt>
@@ -972,13 +1047,22 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1015,9 +1099,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Performance!$C$4:$I$4</c:f>
+              <c:f>Performance!$C$4:$L$4</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Bau</c:v>
                 </c:pt>
@@ -1031,23 +1115,32 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>PyPy</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Rust</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Swift</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$C$9:$I$9</c:f>
+              <c:f>Performance!$C$9:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
@@ -1061,13 +1154,22 @@
                   <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>14.9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3.8</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1239,6 +1341,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1246,7 +1349,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1508,7 +1610,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Swift</c:v>
+                  <c:v>Nim</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1550,16 +1652,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>283</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6566</c:v>
+                  <c:v>6096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2542</c:v>
+                  <c:v>2351</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3195</c:v>
+                  <c:v>3068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1579,7 +1681,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kotlin</c:v>
+                  <c:v>Swift</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1621,16 +1723,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>277</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6953</c:v>
+                  <c:v>6566</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2590</c:v>
+                  <c:v>2542</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3501</c:v>
+                  <c:v>3195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1650,7 +1752,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C</c:v>
+                  <c:v>Vlang</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1695,13 +1797,13 @@
                   <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7268</c:v>
+                  <c:v>6732</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2604</c:v>
+                  <c:v>2740</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3477</c:v>
+                  <c:v>3028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,7 +1823,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Go</c:v>
+                  <c:v>Kotlin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1763,16 +1865,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>334</c:v>
+                  <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7037</c:v>
+                  <c:v>6953</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2764</c:v>
+                  <c:v>2590</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3217</c:v>
+                  <c:v>3501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1780,6 +1882,371 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-DD04-B54E-B7F7-3461ED87B74D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Concise!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Go</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Concise!$C$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Lines</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bytes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Whitespace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alphanumeric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Concise!$C$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7037</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3217</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4F6-E946-8D0D-119611D52763}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Concise!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Concise!$C$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Lines</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bytes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Whitespace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alphanumeric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Concise!$C$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7268</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3477</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F4F6-E946-8D0D-119611D52763}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Concise!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Concise!$C$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Lines</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bytes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Whitespace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alphanumeric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Concise!$C$11:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F4F6-E946-8D0D-119611D52763}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Concise!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rust</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Concise!$C$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Lines</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bytes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Whitespace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alphanumeric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Concise!$C$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8311</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3311</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F4F6-E946-8D0D-119611D52763}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Concise!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zig</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Concise!$C$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Lines</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bytes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Whitespace</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Alphanumeric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Concise!$C$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10678</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3529</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE10-6F45-BF22-CF375864CE78}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1943,6 +2410,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1950,7 +2418,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2101,9 +2568,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Concise!$I$3:$I$10</c:f>
+              <c:f>Concise!$I$3:$I$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Python</c:v>
                 </c:pt>
@@ -2111,32 +2578,41 @@
                   <c:v>Bau</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Swift</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Kotlin</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>C</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Go</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Rust</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Concise!$J$3:$J$10</c:f>
+              <c:f>Concise!$J$3:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2144,22 +2620,31 @@
                   <c:v>1.0225225225225225</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.1351351351351351</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.2747747747747749</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2477477477477477</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.3783783783783783</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.2477477477477477</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.5045045045045045</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>1.3783783783783783</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1.2522522522522523</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1.5315315315315314</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6936936936936937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2196,9 +2681,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Concise!$I$3:$I$10</c:f>
+              <c:f>Concise!$I$3:$I$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Python</c:v>
                 </c:pt>
@@ -2206,32 +2691,41 @@
                   <c:v>Bau</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Swift</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Kotlin</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>C</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Go</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Rust</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Concise!$K$3:$K$10</c:f>
+              <c:f>Concise!$K$3:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2239,22 +2733,31 @@
                   <c:v>1.0014792899408285</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.1272189349112425</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.2141272189349113</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>1.2448224852071006</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.2856878698224852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>1.3012204142011834</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.3439349112426036</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3012204142011834</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>1.4659763313609466</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1.5367973372781065</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9744822485207101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,9 +2794,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Concise!$I$3:$I$10</c:f>
+              <c:f>Concise!$I$3:$I$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Python</c:v>
                 </c:pt>
@@ -2301,32 +2804,41 @@
                   <c:v>Bau</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Swift</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Kotlin</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>C</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Go</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Rust</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Concise!$L$3:$L$10</c:f>
+              <c:f>Concise!$L$3:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2334,22 +2846,31 @@
                   <c:v>0.98897411313518691</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.1270373921380632</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.2186001917545541</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>1.3135186960690315</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.2416107382550334</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>1.3250239693192714</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.2483221476510067</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3250239693192714</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>1.592521572387344</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1.587248322147651</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6917545541706616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2386,9 +2907,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Concise!$I$3:$I$10</c:f>
+              <c:f>Concise!$I$3:$I$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Python</c:v>
                 </c:pt>
@@ -2396,32 +2917,41 @@
                   <c:v>Bau</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Swift</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Kotlin</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>C</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Go</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Rust</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Concise!$M$3:$M$10</c:f>
+              <c:f>Concise!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2429,22 +2959,31 @@
                   <c:v>1.0466281310211947</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.1822736030828516</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.23121387283237</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>1.166859344894027</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.3491329479768785</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>1.2396917148362234</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.3398843930635838</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2396917148362234</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>1.3876685934489403</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1.4231213872832371</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0809248554913293</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2481,9 +3020,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Concise!$I$3:$I$10</c:f>
+              <c:f>Concise!$I$3:$I$13</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Python</c:v>
                 </c:pt>
@@ -2491,32 +3030,41 @@
                   <c:v>Bau</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Nim</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Swift</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>Vlang</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Kotlin</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>C</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Go</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Rust</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Zig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Concise!$N$3:$N$10</c:f>
+              <c:f>Concise!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2524,22 +3072,31 @@
                   <c:v>0.93814432989690721</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.99263622974963184</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.2268041237113403</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>1.3019145802650958</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.2739322533136965</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>1.5022091310751104</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.6583210603829159</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5022091310751104</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>1.4830633284241532</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1.8335787923416789</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5493372606774667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2695,7 +3252,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2713,6 +3270,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2720,7 +3278,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4602,15 +5159,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>754317</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>54133</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>373317</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>155733</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4638,15 +5195,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>533260</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>575360</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>98234</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>126298</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>193484</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4993,8 +5550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430266A2-5A9C-AA42-B61E-0693631C31C7}">
   <dimension ref="B4:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5006,33 +5563,42 @@
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -5049,16 +5615,25 @@
         <v>3.4</v>
       </c>
       <c r="G5" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="H5" s="1">
         <v>8.5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>5.9</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -5075,16 +5650,25 @@
         <v>2.1</v>
       </c>
       <c r="G6" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H6" s="1">
         <v>5.2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>2</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -5101,16 +5685,25 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="G7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="1">
         <v>15.4</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>1.8</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -5127,16 +5720,25 @@
         <v>3.5</v>
       </c>
       <c r="G8" s="1">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>1.5</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -5153,25 +5755,68 @@
         <v>3.8</v>
       </c>
       <c r="G9" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H9" s="1">
         <v>14.9</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>3.8</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="L9" s="1">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <f t="shared" ref="C10:I10" si="0">SUM(C5:C9)</f>
+        <v>15.1</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>20.9</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>17.2</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>45.5</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>46.300000000000004</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" ref="J10" si="1">SUM(J5:J9)</f>
+        <v>40.9</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10" si="2">SUM(K5:K9)</f>
+        <v>20.3</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10" si="3">SUM(L5:L9)</f>
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -5180,7 +5825,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -5189,7 +5834,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -5198,7 +5843,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -5207,7 +5852,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -5224,15 +5869,15 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>0.42202546296296295</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>0.4258912037037037</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <f>K18-K17</f>
         <v>3.8657407407407529E-3</v>
       </c>
@@ -5280,6 +5925,1010 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCA3CD0-A1E2-3843-9734-943657D6AF5A}">
+  <dimension ref="B2:U74"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="21" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>222</v>
+      </c>
+      <c r="D3">
+        <v>5408</v>
+      </c>
+      <c r="E3">
+        <v>2086</v>
+      </c>
+      <c r="F3">
+        <v>2595</v>
+      </c>
+      <c r="G3">
+        <v>679</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="str">
+        <f>B3</f>
+        <v>Python</v>
+      </c>
+      <c r="J3">
+        <f>1/C$3*C3</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3" si="0">1/D$3*D3</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3" si="1">1/E$3*E3</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3" si="2">1/F$3*F3</f>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3" si="3">1/G$3*G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>227</v>
+      </c>
+      <c r="D4">
+        <v>5416</v>
+      </c>
+      <c r="E4">
+        <v>2063</v>
+      </c>
+      <c r="F4">
+        <v>2716</v>
+      </c>
+      <c r="G4">
+        <v>637</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="str">
+        <f t="shared" ref="I4:I12" si="4">B4</f>
+        <v>Bau</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J12" si="5">1/C$3*C4</f>
+        <v>1.0225225225225225</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K12" si="6">1/D$3*D4</f>
+        <v>1.0014792899408285</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L12" si="7">1/E$3*E4</f>
+        <v>0.98897411313518691</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M12" si="8">1/F$3*F4</f>
+        <v>1.0466281310211947</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N12" si="9">1/G$3*G4</f>
+        <v>0.93814432989690721</v>
+      </c>
+      <c r="P4">
+        <f>J4-J$3</f>
+        <v>2.2522522522522515E-2</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q12" si="10">K4-K$3</f>
+        <v>1.4792899408284654E-3</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R12" si="11">L4-L$3</f>
+        <v>-1.1025886864813095E-2</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S12" si="12">M4-M$3</f>
+        <v>4.6628131021194674E-2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T12" si="13">N4-N$3</f>
+        <v>-6.1855670103092786E-2</v>
+      </c>
+      <c r="U4">
+        <f>SUM(P4:T4)</f>
+        <v>-2.2516134833602264E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5">
+        <v>252</v>
+      </c>
+      <c r="D5">
+        <v>6096</v>
+      </c>
+      <c r="E5">
+        <v>2351</v>
+      </c>
+      <c r="F5">
+        <v>3068</v>
+      </c>
+      <c r="G5">
+        <v>674</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Nim</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>1.1351351351351351</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>1.1272189349112425</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="7"/>
+        <v>1.1270373921380632</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="8"/>
+        <v>1.1822736030828516</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="9"/>
+        <v>0.99263622974963184</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P12" si="14">J5-J$3</f>
+        <v>0.13513513513513509</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="10"/>
+        <v>0.12721893491124248</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="11"/>
+        <v>0.1270373921380632</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="12"/>
+        <v>0.18227360308285157</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="13"/>
+        <v>-7.3637702503681624E-3</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U12" si="15">SUM(P5:T5)</f>
+        <v>0.56430129501692416</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>283</v>
+      </c>
+      <c r="D6">
+        <v>6566</v>
+      </c>
+      <c r="E6">
+        <v>2542</v>
+      </c>
+      <c r="F6">
+        <v>3195</v>
+      </c>
+      <c r="G6">
+        <v>833</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Swift</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>1.2747747747747749</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>1.2141272189349113</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="7"/>
+        <v>1.2186001917545541</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="8"/>
+        <v>1.23121387283237</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="9"/>
+        <v>1.2268041237113403</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="14"/>
+        <v>0.27477477477477485</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="10"/>
+        <v>0.21412721893491127</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="11"/>
+        <v>0.21860019175455414</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="12"/>
+        <v>0.23121387283237005</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="13"/>
+        <v>0.22680412371134029</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="15"/>
+        <v>1.1655201820079506</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7">
+        <v>306</v>
+      </c>
+      <c r="D7">
+        <v>6732</v>
+      </c>
+      <c r="E7">
+        <v>2740</v>
+      </c>
+      <c r="F7">
+        <v>3028</v>
+      </c>
+      <c r="G7">
+        <v>884</v>
+      </c>
+      <c r="H7">
+        <v>81</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Vlang</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>1.3783783783783783</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>1.2448224852071006</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="7"/>
+        <v>1.3135186960690315</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="8"/>
+        <v>1.166859344894027</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="9"/>
+        <v>1.3019145802650958</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="14"/>
+        <v>0.37837837837837829</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="10"/>
+        <v>0.24482248520710059</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="11"/>
+        <v>0.31351869606903149</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="12"/>
+        <v>0.16685934489402698</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="13"/>
+        <v>0.30191458026509577</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="15"/>
+        <v>1.4054934848136331</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>277</v>
+      </c>
+      <c r="D8">
+        <v>6953</v>
+      </c>
+      <c r="E8">
+        <v>2590</v>
+      </c>
+      <c r="F8">
+        <v>3501</v>
+      </c>
+      <c r="G8">
+        <v>865</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Kotlin</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>1.2477477477477477</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>1.2856878698224852</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>1.2416107382550334</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="8"/>
+        <v>1.3491329479768785</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="9"/>
+        <v>1.2739322533136965</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="14"/>
+        <v>0.24774774774774766</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="10"/>
+        <v>0.28568786982248517</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="11"/>
+        <v>0.24161073825503343</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="12"/>
+        <v>0.34913294797687855</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="13"/>
+        <v>0.27393225331369653</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="15"/>
+        <v>1.3981115571158413</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>334</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7037</v>
+      </c>
+      <c r="E9">
+        <v>2764</v>
+      </c>
+      <c r="F9">
+        <v>3217</v>
+      </c>
+      <c r="G9">
+        <v>1020</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Go</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>1.5045045045045045</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>1.3012204142011834</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="7"/>
+        <v>1.3250239693192714</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="8"/>
+        <v>1.2396917148362234</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="9"/>
+        <v>1.5022091310751104</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="14"/>
+        <v>0.50450450450450446</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="10"/>
+        <v>0.3012204142011834</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="11"/>
+        <v>0.32502396931927136</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="12"/>
+        <v>0.23969171483622342</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="13"/>
+        <v>0.50220913107511045</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="15"/>
+        <v>1.8726497339362931</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>306</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7268</v>
+      </c>
+      <c r="E10">
+        <v>2604</v>
+      </c>
+      <c r="F10">
+        <v>3477</v>
+      </c>
+      <c r="G10">
+        <v>1126</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+      <c r="I10" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>C</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>1.3783783783783783</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>1.3439349112426036</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="7"/>
+        <v>1.2483221476510067</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="8"/>
+        <v>1.3398843930635838</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="9"/>
+        <v>1.6583210603829159</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="14"/>
+        <v>0.37837837837837829</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="10"/>
+        <v>0.34393491124260356</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="11"/>
+        <v>0.24832214765100669</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="12"/>
+        <v>0.33988439306358376</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="13"/>
+        <v>0.65832106038291593</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="15"/>
+        <v>1.9688408907184882</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>278</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7928</v>
+      </c>
+      <c r="E11">
+        <v>3322</v>
+      </c>
+      <c r="F11">
+        <v>3601</v>
+      </c>
+      <c r="G11">
+        <v>1007</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Java</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>1.2522522522522523</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>1.4659763313609466</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="7"/>
+        <v>1.592521572387344</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="8"/>
+        <v>1.3876685934489403</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="9"/>
+        <v>1.4830633284241532</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="14"/>
+        <v>0.25225225225225234</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="10"/>
+        <v>0.46597633136094663</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="11"/>
+        <v>0.59252157238734404</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="12"/>
+        <v>0.38766859344894034</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="13"/>
+        <v>0.48306332842415323</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="15"/>
+        <v>2.1814820778736363</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>340</v>
+      </c>
+      <c r="D12" s="3">
+        <v>8311</v>
+      </c>
+      <c r="E12">
+        <v>3311</v>
+      </c>
+      <c r="F12">
+        <v>3693</v>
+      </c>
+      <c r="G12">
+        <v>1245</v>
+      </c>
+      <c r="H12">
+        <v>65</v>
+      </c>
+      <c r="I12" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Rust</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>1.5315315315315314</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>1.5367973372781065</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="7"/>
+        <v>1.587248322147651</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="8"/>
+        <v>1.4231213872832371</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="9"/>
+        <v>1.8335787923416789</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="14"/>
+        <v>0.53153153153153143</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="10"/>
+        <v>0.53679733727810652</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="11"/>
+        <v>0.58724832214765099</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="12"/>
+        <v>0.42312138728323712</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="13"/>
+        <v>0.83357879234167886</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="15"/>
+        <v>2.9122773705822045</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13">
+        <v>376</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10678</v>
+      </c>
+      <c r="E13">
+        <v>3529</v>
+      </c>
+      <c r="F13">
+        <v>5400</v>
+      </c>
+      <c r="G13">
+        <v>1731</v>
+      </c>
+      <c r="H13">
+        <v>18</v>
+      </c>
+      <c r="I13" s="4" t="str">
+        <f t="shared" ref="I13" si="16">B13</f>
+        <v>Zig</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13" si="17">1/C$3*C13</f>
+        <v>1.6936936936936937</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13" si="18">1/D$3*D13</f>
+        <v>1.9744822485207101</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13" si="19">1/E$3*E13</f>
+        <v>1.6917545541706616</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13" si="20">1/F$3*F13</f>
+        <v>2.0809248554913293</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13" si="21">1/G$3*G13</f>
+        <v>2.5493372606774667</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D43" s="3"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I51" s="3"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I53" s="3"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I54" s="3"/>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I55" s="3"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I57" s="3"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I58" s="3"/>
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I59" s="3"/>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I60" s="3"/>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I61" s="3"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I62" s="3"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I63" s="3"/>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I64" s="3"/>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I65" s="3"/>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I66" s="3"/>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I67" s="3"/>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I68" s="3"/>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I69" s="3"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I74" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCE9842-6C14-0245-8092-DD3DC9C4F639}">
   <dimension ref="A1:J32"/>
   <sheetViews>
@@ -6116,654 +7765,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCA3CD0-A1E2-3843-9734-943657D6AF5A}">
-  <dimension ref="B2:N74"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>222</v>
-      </c>
-      <c r="D3">
-        <v>5408</v>
-      </c>
-      <c r="E3">
-        <v>2086</v>
-      </c>
-      <c r="F3">
-        <v>2595</v>
-      </c>
-      <c r="G3">
-        <v>679</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-      <c r="I3" s="4" t="str">
-        <f>B3</f>
-        <v>Python</v>
-      </c>
-      <c r="J3">
-        <f>1/C$3*C3</f>
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="0">1/D$3*D3</f>
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="1">1/E$3*E3</f>
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M8" si="2">1/F$3*F3</f>
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N8" si="3">1/G$3*G3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>227</v>
-      </c>
-      <c r="D4">
-        <v>5416</v>
-      </c>
-      <c r="E4">
-        <v>2063</v>
-      </c>
-      <c r="F4">
-        <v>2716</v>
-      </c>
-      <c r="G4">
-        <v>637</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4" t="str">
-        <f t="shared" ref="I4:I10" si="4">B4</f>
-        <v>Bau</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J8" si="5">1/C$3*C4</f>
-        <v>1.0225225225225225</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>1.0014792899408285</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="1"/>
-        <v>0.98897411313518691</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
-        <v>1.0466281310211947</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="3"/>
-        <v>0.93814432989690721</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>283</v>
-      </c>
-      <c r="D5">
-        <v>6566</v>
-      </c>
-      <c r="E5">
-        <v>2542</v>
-      </c>
-      <c r="F5">
-        <v>3195</v>
-      </c>
-      <c r="G5">
-        <v>833</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>Swift</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="5"/>
-        <v>1.2747747747747749</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>1.2141272189349113</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
-        <v>1.2186001917545541</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
-        <v>1.23121387283237</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="3"/>
-        <v>1.2268041237113403</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>277</v>
-      </c>
-      <c r="D6">
-        <v>6953</v>
-      </c>
-      <c r="E6">
-        <v>2590</v>
-      </c>
-      <c r="F6">
-        <v>3501</v>
-      </c>
-      <c r="G6">
-        <v>865</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>Kotlin</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="5"/>
-        <v>1.2477477477477477</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1.2856878698224852</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>1.2416107382550334</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
-        <v>1.3491329479768785</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="3"/>
-        <v>1.2739322533136965</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>306</v>
-      </c>
-      <c r="D7">
-        <v>7268</v>
-      </c>
-      <c r="E7">
-        <v>2604</v>
-      </c>
-      <c r="F7">
-        <v>3477</v>
-      </c>
-      <c r="G7">
-        <v>1126</v>
-      </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
-      <c r="I7" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>C</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="5"/>
-        <v>1.3783783783783783</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>1.3439349112426036</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
-        <v>1.2483221476510067</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>1.3398843930635838</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="3"/>
-        <v>1.6583210603829159</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>334</v>
-      </c>
-      <c r="D8">
-        <v>7037</v>
-      </c>
-      <c r="E8">
-        <v>2764</v>
-      </c>
-      <c r="F8">
-        <v>3217</v>
-      </c>
-      <c r="G8">
-        <v>1020</v>
-      </c>
-      <c r="H8">
-        <v>9</v>
-      </c>
-      <c r="I8" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>Go</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="5"/>
-        <v>1.5045045045045045</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>1.3012204142011834</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>1.3250239693192714</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>1.2396917148362234</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="3"/>
-        <v>1.5022091310751104</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>278</v>
-      </c>
-      <c r="D9" s="3">
-        <v>7928</v>
-      </c>
-      <c r="E9">
-        <v>3322</v>
-      </c>
-      <c r="F9">
-        <v>3601</v>
-      </c>
-      <c r="G9">
-        <v>1007</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>Java</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ref="J9" si="6">1/C$3*C9</f>
-        <v>1.2522522522522523</v>
-      </c>
-      <c r="K9">
-        <f t="shared" ref="K9:K10" si="7">1/D$3*D9</f>
-        <v>1.4659763313609466</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ref="L9:L10" si="8">1/E$3*E9</f>
-        <v>1.592521572387344</v>
-      </c>
-      <c r="M9">
-        <f t="shared" ref="M9:M10" si="9">1/F$3*F9</f>
-        <v>1.3876685934489403</v>
-      </c>
-      <c r="N9">
-        <f t="shared" ref="N9:N10" si="10">1/G$3*G9</f>
-        <v>1.4830633284241532</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>340</v>
-      </c>
-      <c r="D10" s="3">
-        <v>8311</v>
-      </c>
-      <c r="E10">
-        <v>3311</v>
-      </c>
-      <c r="F10">
-        <v>3693</v>
-      </c>
-      <c r="G10">
-        <v>1245</v>
-      </c>
-      <c r="H10">
-        <v>65</v>
-      </c>
-      <c r="I10" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>Rust</v>
-      </c>
-      <c r="J10">
-        <f t="shared" ref="J10" si="11">1/C$3*C10</f>
-        <v>1.5315315315315314</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="7"/>
-        <v>1.5367973372781065</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="8"/>
-        <v>1.587248322147651</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="9"/>
-        <v>1.4231213872832371</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="10"/>
-        <v>1.8335787923416789</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D43" s="3"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="K47" s="3"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="K48" s="3"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="K50" s="3"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I52" s="3"/>
-      <c r="K52" s="3"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I54" s="3"/>
-      <c r="K54" s="3"/>
-    </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I55" s="3"/>
-      <c r="K55" s="3"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I56" s="3"/>
-      <c r="K56" s="3"/>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I57" s="3"/>
-      <c r="K57" s="3"/>
-    </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I58" s="3"/>
-      <c r="K58" s="3"/>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I59" s="3"/>
-      <c r="K59" s="3"/>
-    </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I60" s="3"/>
-      <c r="K60" s="3"/>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I61" s="3"/>
-      <c r="K61" s="3"/>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I62" s="3"/>
-      <c r="K62" s="3"/>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I63" s="3"/>
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I64" s="3"/>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I65" s="3"/>
-      <c r="K65" s="3"/>
-    </row>
-    <row r="66" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I66" s="3"/>
-      <c r="K66" s="3"/>
-    </row>
-    <row r="67" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I67" s="3"/>
-      <c r="K67" s="3"/>
-    </row>
-    <row r="68" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I68" s="3"/>
-      <c r="K68" s="3"/>
-    </row>
-    <row r="69" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I69" s="3"/>
-      <c r="K69" s="3"/>
-    </row>
-    <row r="70" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I74" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Stdlib: Int and bigint math improvements; JSON
</commit_message>
<xml_diff>
--- a/doc/performance.xlsx
+++ b/doc/performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mueller/data/bau/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FB8C5C-44B4-C74B-A92F-57BA8C016EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002423A5-19F2-E84A-BACD-D95A574B49B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34040" windowHeight="17500" xr2:uid="{8BA8907E-A4D7-9D46-8614-8210467CB087}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="147">
   <si>
     <t>Benchmark</t>
   </si>
@@ -572,7 +572,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -714,34 +714,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>6.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.6</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,34 +821,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -928,34 +928,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.8</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.4</c:v>
+                  <c:v>10.199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1035,34 +1035,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.6</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1142,34 +1142,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.5</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.9</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.7</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1247,7 +1247,8 @@
         <c:axId val="15769792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16"/>
+          <c:max val="11"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1386,7 +1387,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2455,7 +2456,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5548,10 +5549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430266A2-5A9C-AA42-B61E-0693631C31C7}">
-  <dimension ref="B4:N23"/>
+  <dimension ref="B4:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5563,7 +5564,7 @@
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -5597,226 +5598,272 @@
       <c r="L4" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="N4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>5.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="D5" s="1">
-        <v>5.0999999999999996</v>
+        <v>3.3</v>
       </c>
       <c r="E5" s="1">
-        <v>11</v>
+        <v>6.7</v>
       </c>
       <c r="F5" s="1">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
-        <v>5.2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="I5" s="1">
-        <v>5.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="J5" s="1">
-        <v>12</v>
+        <v>10.8</v>
       </c>
       <c r="K5" s="1">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="L5" s="1">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+        <v>4.5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>67</v>
+      </c>
+      <c r="O5">
+        <f>N5/H5</f>
+        <v>12.181818181818182</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="D6" s="1">
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="E6" s="1">
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="F6" s="1">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="G6" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="H6" s="1">
-        <v>5.2</v>
+        <v>3.7</v>
       </c>
       <c r="I6" s="1">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="J6" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="K6" s="1">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="L6" s="1">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+        <v>1.6</v>
+      </c>
+      <c r="N6" s="1">
+        <v>51</v>
+      </c>
+      <c r="O6">
+        <f>N6/H6</f>
+        <v>13.783783783783782</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="D7" s="1">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="E7" s="1">
-        <v>3.2</v>
+        <v>1.9</v>
       </c>
       <c r="F7" s="1">
-        <v>4.4000000000000004</v>
+        <v>2.7</v>
       </c>
       <c r="G7" s="1">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="H7" s="1">
-        <v>15.4</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="I7" s="1">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="J7" s="1">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="K7" s="1">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="L7" s="1">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>143</v>
+      </c>
+      <c r="O7">
+        <f>N7/H7</f>
+        <v>14.019607843137257</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>2.6</v>
+        <v>1.3</v>
       </c>
       <c r="D8" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="I8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="G8" s="1">
-        <v>32</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1.5</v>
-      </c>
       <c r="J8" s="1">
-        <v>7.7</v>
+        <v>5</v>
       </c>
       <c r="K8" s="1">
-        <v>5.3</v>
+        <v>3.2</v>
       </c>
       <c r="L8" s="1">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+        <v>3.1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="O8">
+        <f>N8/H8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>3.5</v>
+        <v>1.8</v>
       </c>
       <c r="D9" s="1">
-        <v>3.5</v>
+        <v>1.8</v>
       </c>
       <c r="E9" s="1">
-        <v>3.5</v>
+        <v>1.8</v>
       </c>
       <c r="F9" s="1">
-        <v>3.8</v>
+        <v>2.1</v>
       </c>
       <c r="G9" s="1">
-        <v>3.5</v>
+        <v>1.9</v>
       </c>
       <c r="H9" s="1">
-        <v>14.9</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I9" s="1">
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1">
-        <v>17</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="K9" s="1">
-        <v>3.6</v>
+        <v>1.8</v>
       </c>
       <c r="L9" s="1">
-        <v>15.7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+        <v>9.4</v>
+      </c>
+      <c r="N9" s="1">
+        <v>129</v>
+      </c>
+      <c r="O9">
+        <f>N9/H9</f>
+        <v>13.163265306122447</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1">
         <f t="shared" ref="C10:I10" si="0">SUM(C5:C9)</f>
-        <v>15.1</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>13.1</v>
+        <v>8.2000000000000011</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>20.9</v>
+        <v>12.5</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>17.2</v>
+        <v>10.5</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>45.5</v>
+        <v>33</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>46.300000000000004</v>
+        <v>30.599999999999998</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" ref="J10" si="1">SUM(J5:J9)</f>
-        <v>40.9</v>
+        <v>28.7</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" ref="K10" si="2">SUM(K5:K9)</f>
-        <v>20.3</v>
+        <v>12.3</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" ref="L10" si="3">SUM(L5:L9)</f>
-        <v>31.7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L10:N10" si="3">SUM(L5:L9)</f>
+        <v>19.8</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="3"/>
+        <v>392.8</v>
+      </c>
+      <c r="O10">
+        <f>N10/H10</f>
+        <v>12.836601307189543</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -5825,7 +5872,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -5834,7 +5881,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -5843,7 +5890,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -5852,7 +5899,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>